<commit_message>
Sort Data (value, color,icon, unsort)
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://comhlamh-my.sharepoint.com/personal/grace_comhlamh_org/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/halanbm/Documents/excel-journey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B57C583-44B8-4588-8BCB-F31BDE77F664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5CAC718-75DF-9A42-B815-6CF26D308372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{51A40A1C-2FDD-4C9F-8189-954237FD9E7E}"/>
+    <workbookView xWindow="32340" yWindow="-8540" windowWidth="42080" windowHeight="26140" activeTab="1" xr2:uid="{51A40A1C-2FDD-4C9F-8189-954237FD9E7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro+Absolute-relative-mix" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Cell modes  R,E,P,E'!$B$10:$E$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Cell modes  R,E,P,E'!$C$10:$C$25</definedName>
+    <definedName name="_xlnm.Extract" localSheetId="1">'Cell modes  R,E,P,E'!$C$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="55">
   <si>
     <t>Jan</t>
   </si>
@@ -164,6 +164,48 @@
   </si>
   <si>
     <t>SUMAR CUANDO HAY UN FILTRO ASI NO SUMA TODO LAS COLUMNAS</t>
+  </si>
+  <si>
+    <t>funtion SUBTOTAL is for an action when do you filter a table and you want just do the action to the filter results</t>
+  </si>
+  <si>
+    <t>ADVANCE FILTERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> YOU PUT THEM IN SEPARATE CELLS</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>*pants*</t>
+  </si>
+  <si>
+    <t>that contains the word pants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt; </t>
+  </si>
+  <si>
+    <t>means !=</t>
+  </si>
+  <si>
+    <t>typing below is OR condition</t>
+  </si>
+  <si>
+    <t>typing beside is AND condition</t>
+  </si>
+  <si>
+    <t>&gt;200</t>
+  </si>
+  <si>
+    <t>&lt;400</t>
+  </si>
+  <si>
+    <t>Copy the unique results of the conditions that you made</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -321,20 +363,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -356,23 +389,36 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="4">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <border outline="0">
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -382,27 +428,13 @@
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF4EA72E"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -418,12 +450,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DE36F16-D120-40F4-A205-6343169F2922}" name="Table1" displayName="Table1" ref="B10:E25" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="2" tableBorderDxfId="3">
-  <autoFilter ref="B10:E25" xr:uid="{6DE36F16-D120-40F4-A205-6343169F2922}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6DE36F16-D120-40F4-A205-6343169F2922}" name="Table1" displayName="Table1" ref="B10:E25" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3333EA48-548B-43D8-9D13-9A9C883661DF}" name="Chanel"/>
     <tableColumn id="2" xr3:uid="{11CBEDEB-47B5-4C74-BBF7-EC5D50CB9A1D}" name="Product"/>
-    <tableColumn id="3" xr3:uid="{471202CC-B8B5-4040-8D12-BB2BA44700A4}" name="date" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{471202CC-B8B5-4040-8D12-BB2BA44700A4}" name="date" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{33DE968C-20C2-48DA-9EC4-85E7ED9C8A6F}" name="sales value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -750,30 +781,30 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="5" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+    </row>
+    <row r="2" spans="1:14" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -794,7 +825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -817,7 +848,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -840,7 +871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -863,7 +894,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -886,24 +917,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="J8" s="5" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="J8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>11</v>
       </c>
@@ -932,7 +963,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -952,31 +983,31 @@
         <f>SUM(B11:E11)</f>
         <v>1100</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <f>F11/$F$14</f>
         <v>0.4408817635270541</v>
       </c>
       <c r="J11" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <f>B11/$F11</f>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <f t="shared" ref="L11:N13" si="0">C11/$F11</f>
         <v>0.18181818181818182</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="3">
         <f t="shared" si="0"/>
         <v>0.45454545454545453</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="3">
         <f t="shared" si="0"/>
         <v>0.27272727272727271</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -996,31 +1027,31 @@
         <f t="shared" ref="F12:F13" si="1">SUM(B12:E12)</f>
         <v>630</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <f t="shared" ref="G12:G13" si="2">F12/$F$14</f>
         <v>0.25250501002004005</v>
       </c>
       <c r="J12" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <f t="shared" ref="K12:K13" si="3">B12/$F12</f>
         <v>0.23809523809523808</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="3">
         <f t="shared" ref="L12:L13" si="4">C12/$F12</f>
         <v>0.3968253968253968</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="3">
         <f t="shared" ref="M12:M13" si="5">D12/$F12</f>
         <v>0.22222222222222221</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="3">
         <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1040,31 +1071,31 @@
         <f t="shared" si="1"/>
         <v>765</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <f t="shared" si="2"/>
         <v>0.30661322645290578</v>
       </c>
       <c r="J13" t="s">
         <v>18</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="3">
         <f t="shared" si="3"/>
         <v>0.30065359477124182</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="3">
         <f t="shared" si="4"/>
         <v>0.45751633986928103</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="3">
         <f t="shared" si="5"/>
         <v>0.13071895424836602</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="3">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="F14">
         <f>SUM(F11:F13)</f>
         <v>2495</v>
@@ -1083,86 +1114,94 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E84FC36C-FDB7-44DA-A84F-ED6DFC77365A}">
-  <dimension ref="A3:N25"/>
+  <dimension ref="A2:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:E25"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.83203125" customWidth="1"/>
     <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5" customWidth="1"/>
+    <col min="17" max="17" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="2" spans="1:17" ht="64" x14ac:dyDescent="0.2">
+      <c r="Q2" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-    </row>
-    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+    </row>
+    <row r="8" spans="1:17" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="14" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+    </row>
+    <row r="10" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="8">
         <v>43313</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="10">
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="8">
         <v>43313</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="9">
         <v>250</v>
       </c>
       <c r="G12" t="s">
@@ -1172,32 +1211,33 @@
         <f>SUM(E12:E25)</f>
         <v>4286</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J12" s="16"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>29</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="8">
         <v>43405</v>
       </c>
       <c r="E13">
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="8">
         <v>43375</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="10">
         <v>260</v>
       </c>
       <c r="G14" t="s">
@@ -1208,14 +1248,14 @@
         <v>4286</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="8">
         <v>43375</v>
       </c>
       <c r="E15">
@@ -1225,7 +1265,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>31</v>
       </c>
@@ -1235,53 +1275,53 @@
       <c r="D16" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="9">
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>28</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="8">
         <v>42746</v>
       </c>
       <c r="E17">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="8">
         <v>42746</v>
       </c>
       <c r="E18">
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>31</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="8">
         <v>42746</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="10">
         <v>410</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>28</v>
       </c>
@@ -1295,7 +1335,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>30</v>
       </c>
@@ -1309,7 +1349,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>28</v>
       </c>
@@ -1319,50 +1359,152 @@
       <c r="D22" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="9">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>28</v>
       </c>
       <c r="C23" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="11">
+      <c r="D23" s="8">
         <v>43313</v>
       </c>
       <c r="E23">
         <v>401</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H23" s="16"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>30</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="11">
+      <c r="D24" s="8">
         <v>43313</v>
       </c>
       <c r="E24">
         <v>430</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>28</v>
       </c>
       <c r="C25" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="8">
         <v>43313</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="10">
         <v>285</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" t="s">
+        <v>44</v>
+      </c>
+      <c r="G29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
+      </c>
+      <c r="G30" t="s">
+        <v>51</v>
+      </c>
+      <c r="H30" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>33</v>
+      </c>
+      <c r="G31" t="s">
+        <v>51</v>
+      </c>
+      <c r="H31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1385,37 +1527,37 @@
       <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="11">
+      <c r="C2" s="8">
         <v>43313</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="9">
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1425,11 +1567,11 @@
       <c r="C3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="9">
         <v>280</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1439,7 +1581,7 @@
       <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>100</v>
       </c>
     </row>

</xml_diff>